<commit_message>
edit code2b.py and data.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Mô hình hoá\Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\binh1\OneDrive\Desktop\Binh\HK3\MHH\BTL\team\Mathematical_Modelling_Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9FC7715-3826-43D9-AB2A-6A95D493183C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11316"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
   <si>
     <t>capCO2Top</t>
   </si>
@@ -121,12 +120,6 @@
   </si>
   <si>
     <t>MCH2O</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>R</t>
   </si>
   <si>
     <t>CBuf</t>
@@ -213,7 +206,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -541,69 +534,69 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AQ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AO6" sqref="AO6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" style="2" customWidth="1"/>
     <col min="11" max="11" width="9" style="2" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="2" customWidth="1"/>
-    <col min="13" max="14" width="7.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" style="2" customWidth="1"/>
+    <col min="13" max="14" width="7.6640625" style="2" customWidth="1"/>
     <col min="15" max="15" width="8" style="2" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="7.140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="7.109375" style="2" customWidth="1"/>
     <col min="18" max="18" width="7" style="2" customWidth="1"/>
-    <col min="19" max="19" width="6.42578125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="6.5703125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="12.140625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="12.85546875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="6.44140625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="6.5546875" style="2" customWidth="1"/>
+    <col min="21" max="21" width="12.109375" style="2" customWidth="1"/>
+    <col min="22" max="22" width="12.88671875" style="2" customWidth="1"/>
     <col min="23" max="23" width="6" style="2" customWidth="1"/>
-    <col min="24" max="24" width="7.42578125" style="2" customWidth="1"/>
-    <col min="25" max="25" width="7.140625" style="2" customWidth="1"/>
-    <col min="26" max="26" width="7.85546875" style="2" customWidth="1"/>
-    <col min="27" max="27" width="9.140625" style="2"/>
-    <col min="28" max="28" width="6.5703125" style="2" customWidth="1"/>
-    <col min="29" max="29" width="12.28515625" style="2" customWidth="1"/>
-    <col min="30" max="30" width="7.42578125" style="2" customWidth="1"/>
-    <col min="31" max="33" width="9.140625" style="2"/>
-    <col min="34" max="34" width="14.85546875" style="2" customWidth="1"/>
-    <col min="35" max="35" width="9.140625" style="2"/>
-    <col min="36" max="36" width="10.140625" style="2" customWidth="1"/>
-    <col min="37" max="37" width="13.5703125" style="2" customWidth="1"/>
-    <col min="38" max="38" width="14.140625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="7.44140625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="7.109375" style="2" customWidth="1"/>
+    <col min="26" max="26" width="7.88671875" style="2" customWidth="1"/>
+    <col min="27" max="27" width="9.109375" style="2"/>
+    <col min="28" max="28" width="6.5546875" style="2" customWidth="1"/>
+    <col min="29" max="29" width="12.33203125" style="2" customWidth="1"/>
+    <col min="30" max="30" width="7.44140625" style="2" customWidth="1"/>
+    <col min="31" max="33" width="9.109375" style="2"/>
+    <col min="34" max="34" width="14.88671875" style="2" customWidth="1"/>
+    <col min="35" max="35" width="9.109375" style="2"/>
+    <col min="36" max="36" width="10.109375" style="2" customWidth="1"/>
+    <col min="37" max="37" width="13.5546875" style="2" customWidth="1"/>
+    <col min="38" max="38" width="14.109375" style="2" customWidth="1"/>
     <col min="39" max="39" width="10" style="2" customWidth="1"/>
-    <col min="40" max="42" width="9.140625" style="2"/>
+    <col min="40" max="42" width="9.109375" style="2"/>
     <col min="43" max="43" width="10" style="2" customWidth="1"/>
-    <col min="44" max="44" width="6.7109375" style="2" customWidth="1"/>
-    <col min="45" max="45" width="6.28515625" style="2" customWidth="1"/>
-    <col min="46" max="16384" width="9.140625" style="2"/>
+    <col min="44" max="44" width="6.6640625" style="2" customWidth="1"/>
+    <col min="45" max="45" width="6.33203125" style="2" customWidth="1"/>
+    <col min="46" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:43" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -615,13 +608,13 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>3</v>
@@ -672,7 +665,7 @@
         <v>18</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>19</v>
@@ -711,27 +704,21 @@
         <v>30</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="AO1" s="1" t="s">
         <v>31</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AS1" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2">
         <v>480</v>
@@ -791,10 +778,10 @@
         <v>1.52</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="W2" s="2">
         <v>0.75</v>
@@ -830,7 +817,7 @@
         <v>1E-4</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AI2" s="2">
         <v>0.5</v>
@@ -845,13 +832,13 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AM2" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AN2" s="2">
         <v>0.68</v>
       </c>
       <c r="AO2" s="2">
-        <v>30</v>
+        <v>0.03</v>
       </c>
       <c r="AP2" s="2">
         <v>0</v>
@@ -859,16 +846,10 @@
       <c r="AQ2" s="2">
         <v>20000</v>
       </c>
-      <c r="AR2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AS2" s="2" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3">
         <v>495</v>
@@ -928,10 +909,10 @@
         <v>1.34</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="W3" s="2">
         <v>0.75</v>
@@ -967,7 +948,7 @@
         <v>1E-4</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AI3" s="2">
         <v>0.5</v>
@@ -982,13 +963,13 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AM3" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AN3" s="2">
         <v>0.68</v>
       </c>
       <c r="AO3" s="2">
-        <v>30</v>
+        <v>0.03</v>
       </c>
       <c r="AP3" s="2">
         <v>0</v>
@@ -996,16 +977,10 @@
       <c r="AQ3" s="2">
         <v>20000</v>
       </c>
-      <c r="AR3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AS3" s="2" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B4">
         <v>491</v>
@@ -1065,10 +1040,10 @@
         <v>1.4</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="W4" s="2">
         <v>0.75</v>
@@ -1104,7 +1079,7 @@
         <v>1E-4</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AI4" s="2">
         <v>0.7</v>
@@ -1119,13 +1094,13 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AM4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AN4" s="2">
         <v>0.97</v>
       </c>
       <c r="AO4" s="2">
-        <v>30</v>
+        <v>0.03</v>
       </c>
       <c r="AP4" s="2">
         <v>0</v>
@@ -1133,16 +1108,10 @@
       <c r="AQ4" s="2">
         <v>20000</v>
       </c>
-      <c r="AR4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AS4" s="2" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <v>506</v>
@@ -1202,10 +1171,10 @@
         <v>1.42</v>
       </c>
       <c r="U5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="W5" s="2">
         <v>0.75</v>
@@ -1241,7 +1210,7 @@
         <v>1E-4</v>
       </c>
       <c r="AH5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AI5" s="2">
         <v>0.7</v>
@@ -1256,13 +1225,13 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AM5" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AN5" s="2">
         <v>0.97</v>
       </c>
       <c r="AO5" s="2">
-        <v>30</v>
+        <v>0.03</v>
       </c>
       <c r="AP5" s="2">
         <v>0</v>
@@ -1270,16 +1239,10 @@
       <c r="AQ5" s="2">
         <v>20000</v>
       </c>
-      <c r="AR5" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AS5" s="2" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B6">
         <v>478</v>
@@ -1339,10 +1302,10 @@
         <v>1.2250000000000001</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="W6" s="2">
         <v>0.75</v>
@@ -1378,7 +1341,7 @@
         <v>1E-4</v>
       </c>
       <c r="AH6" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AI6" s="2">
         <v>0.4</v>
@@ -1393,13 +1356,13 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AM6" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="AN6" s="2">
         <v>0.97</v>
       </c>
       <c r="AO6" s="2">
-        <v>30</v>
+        <v>0.03</v>
       </c>
       <c r="AP6" s="2">
         <v>0</v>
@@ -1407,79 +1370,73 @@
       <c r="AQ6" s="2">
         <v>20000</v>
       </c>
-      <c r="AR6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AS6" s="2" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="AL7" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL7" s="2" t="s">
+      <c r="AN7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AP7" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AN7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP7" s="2" t="s">
-        <v>55</v>
-      </c>
       <c r="AQ7" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add LAI in data.xlsx
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11316"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6228"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
     <t>capCO2Top</t>
   </si>
@@ -65,12 +65,6 @@
     <t>pTop</t>
   </si>
   <si>
-    <t>fVentSide</t>
-  </si>
-  <si>
-    <t>fVentForced</t>
-  </si>
-  <si>
     <t>Cd</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>ARoof</t>
   </si>
   <si>
-    <t>Uside</t>
-  </si>
-  <si>
     <t>g</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
     <t>cleakage</t>
   </si>
   <si>
-    <t>fVentRoofSide</t>
-  </si>
-  <si>
     <t>nSide</t>
   </si>
   <si>
@@ -201,6 +189,21 @@
   </si>
   <si>
     <t>mg m^-3 s^-1</t>
+  </si>
+  <si>
+    <t>USide</t>
+  </si>
+  <si>
+    <t>TOut</t>
+  </si>
+  <si>
+    <t>nRoof</t>
+  </si>
+  <si>
+    <t>nRoof_Thr</t>
+  </si>
+  <si>
+    <t>LAI</t>
   </si>
 </sst>
 </file>
@@ -535,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ7"/>
+  <dimension ref="A1:AR7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
-      <selection activeCell="AO6" sqref="AO6"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -557,46 +560,40 @@
     <col min="13" max="14" width="7.6640625" style="2" customWidth="1"/>
     <col min="15" max="15" width="8" style="2" customWidth="1"/>
     <col min="16" max="16" width="18.33203125" style="2" customWidth="1"/>
-    <col min="17" max="17" width="7.109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="7" style="2" customWidth="1"/>
-    <col min="19" max="19" width="6.44140625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="6.5546875" style="2" customWidth="1"/>
-    <col min="21" max="21" width="12.109375" style="2" customWidth="1"/>
-    <col min="22" max="22" width="12.88671875" style="2" customWidth="1"/>
-    <col min="23" max="23" width="6" style="2" customWidth="1"/>
-    <col min="24" max="24" width="7.44140625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="7.109375" style="2" customWidth="1"/>
-    <col min="26" max="26" width="7.88671875" style="2" customWidth="1"/>
-    <col min="27" max="27" width="9.109375" style="2"/>
-    <col min="28" max="28" width="6.5546875" style="2" customWidth="1"/>
-    <col min="29" max="29" width="12.33203125" style="2" customWidth="1"/>
-    <col min="30" max="30" width="7.44140625" style="2" customWidth="1"/>
-    <col min="31" max="33" width="9.109375" style="2"/>
-    <col min="34" max="34" width="14.88671875" style="2" customWidth="1"/>
-    <col min="35" max="35" width="9.109375" style="2"/>
-    <col min="36" max="36" width="10.109375" style="2" customWidth="1"/>
+    <col min="17" max="18" width="7.109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="7" style="2" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="6.5546875" style="2" customWidth="1"/>
+    <col min="22" max="22" width="6" style="2" customWidth="1"/>
+    <col min="23" max="23" width="7.44140625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="7.109375" style="2" customWidth="1"/>
+    <col min="25" max="25" width="7.88671875" style="2" customWidth="1"/>
+    <col min="26" max="26" width="9.109375" style="2"/>
+    <col min="27" max="27" width="6.5546875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="12.33203125" style="2" customWidth="1"/>
+    <col min="29" max="29" width="7.44140625" style="2" customWidth="1"/>
+    <col min="30" max="33" width="9.109375" style="2"/>
+    <col min="34" max="36" width="10.109375" style="2" customWidth="1"/>
     <col min="37" max="37" width="13.5546875" style="2" customWidth="1"/>
     <col min="38" max="38" width="14.109375" style="2" customWidth="1"/>
     <col min="39" max="39" width="10" style="2" customWidth="1"/>
     <col min="40" max="42" width="9.109375" style="2"/>
     <col min="43" max="43" width="10" style="2" customWidth="1"/>
-    <col min="44" max="44" width="6.6640625" style="2" customWidth="1"/>
-    <col min="45" max="45" width="6.33203125" style="2" customWidth="1"/>
-    <col min="46" max="16384" width="9.109375" style="2"/>
+    <col min="44" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -608,13 +605,13 @@
         <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>3</v>
@@ -638,87 +635,90 @@
         <v>9</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AO1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AM1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
-        <v>33</v>
+      <c r="AR1" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B2">
         <v>480</v>
@@ -766,58 +766,61 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="Q2" s="2">
-        <v>290</v>
+        <f>6.2+278</f>
+        <v>284.2</v>
       </c>
       <c r="R2" s="2">
-        <v>300</v>
+        <f>15.2+273</f>
+        <v>288.2</v>
       </c>
       <c r="S2" s="2">
+        <f>6.2+278</f>
+        <v>284.2</v>
+      </c>
+      <c r="T2" s="2">
         <v>1.2250000000000001</v>
       </c>
-      <c r="T2" s="2">
+      <c r="U2" s="2">
         <v>1.52</v>
       </c>
-      <c r="U2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>43</v>
+      <c r="V2" s="2">
+        <v>0.75</v>
       </c>
       <c r="W2" s="2">
-        <v>0.75</v>
+        <v>0.4</v>
       </c>
       <c r="X2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="Y2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>9.81</v>
+      </c>
+      <c r="AB2" s="2">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="AD2" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="AE2" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF2" s="2">
+        <v>1E-4</v>
+      </c>
+      <c r="AG2" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="AH2" s="2">
         <v>0.4</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>0.1</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>9.81</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>3</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>2.9</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>1</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="AH2" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="AI2" s="2">
         <v>0.5</v>
@@ -832,7 +835,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AM2" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AN2" s="2">
         <v>0.68</v>
@@ -846,10 +849,13 @@
       <c r="AQ2" s="2">
         <v>20000</v>
       </c>
+      <c r="AR2" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>495</v>
@@ -897,58 +903,60 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="Q3" s="2">
-        <v>288</v>
+        <f xml:space="preserve"> 5.3+273</f>
+        <v>278.3</v>
       </c>
       <c r="R3" s="2">
-        <v>301</v>
+        <v>278.89999999999998</v>
       </c>
       <c r="S3" s="2">
+        <f xml:space="preserve"> 5.3+273</f>
+        <v>278.3</v>
+      </c>
+      <c r="T3" s="2">
         <v>1.22</v>
       </c>
-      <c r="T3" s="2">
+      <c r="U3" s="2">
         <v>1.34</v>
       </c>
-      <c r="U3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>43</v>
+      <c r="V3" s="2">
+        <v>0.75</v>
       </c>
       <c r="W3" s="2">
-        <v>0.75</v>
+        <v>0.45</v>
       </c>
       <c r="X3" s="2">
-        <v>0.45</v>
+        <v>0.1</v>
       </c>
       <c r="Y3" s="2">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="Z3" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AA3" s="2">
-        <v>0</v>
+        <v>9.81</v>
       </c>
       <c r="AB3" s="2">
-        <v>9.81</v>
+        <v>3</v>
       </c>
       <c r="AC3" s="2">
-        <v>3</v>
+        <v>0.12</v>
       </c>
       <c r="AD3" s="2">
-        <v>0.12</v>
+        <v>3.3</v>
       </c>
       <c r="AE3" s="2">
-        <v>3.3</v>
+        <v>1</v>
       </c>
       <c r="AF3" s="2">
-        <v>1</v>
+        <v>1E-4</v>
       </c>
       <c r="AG3" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="AH3" s="2" t="s">
-        <v>43</v>
+        <v>0.5</v>
+      </c>
+      <c r="AH3" s="2">
+        <v>0.6</v>
       </c>
       <c r="AI3" s="2">
         <v>0.5</v>
@@ -963,7 +971,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AM3" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AN3" s="2">
         <v>0.68</v>
@@ -977,10 +985,13 @@
       <c r="AQ3" s="2">
         <v>20000</v>
       </c>
+      <c r="AR3" s="2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>491</v>
@@ -1028,58 +1039,60 @@
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="Q4" s="2">
-        <v>273</v>
+        <f xml:space="preserve"> 6+273</f>
+        <v>279</v>
       </c>
       <c r="R4" s="2">
-        <v>289</v>
+        <v>278.39999999999998</v>
       </c>
       <c r="S4" s="2">
+        <f xml:space="preserve"> 6+273</f>
+        <v>279</v>
+      </c>
+      <c r="T4" s="2">
         <v>1.32</v>
       </c>
-      <c r="T4" s="2">
+      <c r="U4" s="2">
         <v>1.4</v>
       </c>
-      <c r="U4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>43</v>
+      <c r="V4" s="2">
+        <v>0.75</v>
       </c>
       <c r="W4" s="2">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="X4" s="2">
-        <v>0.5</v>
+        <v>0.18</v>
       </c>
       <c r="Y4" s="2">
-        <v>0.18</v>
+        <v>0.5</v>
       </c>
       <c r="Z4" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="2">
-        <v>0</v>
+        <v>9.81</v>
       </c>
       <c r="AB4" s="2">
-        <v>9.81</v>
+        <v>3</v>
       </c>
       <c r="AC4" s="2">
-        <v>3</v>
+        <v>0.12</v>
       </c>
       <c r="AD4" s="2">
-        <v>0.12</v>
+        <v>2.9</v>
       </c>
       <c r="AE4" s="2">
-        <v>2.9</v>
+        <v>1</v>
       </c>
       <c r="AF4" s="2">
-        <v>1</v>
+        <v>1E-4</v>
       </c>
       <c r="AG4" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="AH4" s="2" t="s">
-        <v>43</v>
+        <v>0.7</v>
+      </c>
+      <c r="AH4" s="2">
+        <v>0.65</v>
       </c>
       <c r="AI4" s="2">
         <v>0.7</v>
@@ -1094,7 +1107,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AM4" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AN4" s="2">
         <v>0.97</v>
@@ -1108,10 +1121,13 @@
       <c r="AQ4" s="2">
         <v>20000</v>
       </c>
+      <c r="AR4" s="2">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B5">
         <v>506</v>
@@ -1159,58 +1175,60 @@
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="Q5" s="2">
-        <v>280</v>
+        <f>6.8+273</f>
+        <v>279.8</v>
       </c>
       <c r="R5" s="2">
-        <v>300</v>
+        <v>296.89999999999998</v>
       </c>
       <c r="S5" s="2">
+        <f>6.8+273</f>
+        <v>279.8</v>
+      </c>
+      <c r="T5" s="2">
         <v>1.3149999999999999</v>
       </c>
-      <c r="T5" s="2">
+      <c r="U5" s="2">
         <v>1.42</v>
       </c>
-      <c r="U5" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>43</v>
+      <c r="V5" s="2">
+        <v>0.75</v>
       </c>
       <c r="W5" s="2">
-        <v>0.75</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="X5" s="2">
-        <v>0.55000000000000004</v>
+        <v>0.18</v>
       </c>
       <c r="Y5" s="2">
-        <v>0.18</v>
+        <v>0.5</v>
       </c>
       <c r="Z5" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AA5" s="2">
-        <v>0</v>
+        <v>9.81</v>
       </c>
       <c r="AB5" s="2">
-        <v>9.81</v>
+        <v>3</v>
       </c>
       <c r="AC5" s="2">
-        <v>3</v>
+        <v>0.12</v>
       </c>
       <c r="AD5" s="2">
-        <v>0.12</v>
+        <v>2.9</v>
       </c>
       <c r="AE5" s="2">
-        <v>2.9</v>
+        <v>1</v>
       </c>
       <c r="AF5" s="2">
-        <v>1</v>
+        <v>1E-4</v>
       </c>
       <c r="AG5" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="AH5" s="2" t="s">
-        <v>43</v>
+        <v>0.7</v>
+      </c>
+      <c r="AH5" s="2">
+        <v>0.7</v>
       </c>
       <c r="AI5" s="2">
         <v>0.7</v>
@@ -1225,7 +1243,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AM5" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AN5" s="2">
         <v>0.97</v>
@@ -1239,10 +1257,13 @@
       <c r="AQ5" s="2">
         <v>20000</v>
       </c>
+      <c r="AR5" s="2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>478</v>
@@ -1290,58 +1311,61 @@
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="Q6" s="2">
-        <v>281</v>
+        <f>6.8+273</f>
+        <v>279.8</v>
       </c>
       <c r="R6" s="2">
-        <v>299</v>
+        <f>15.7+273</f>
+        <v>288.7</v>
       </c>
       <c r="S6" s="2">
+        <f>6.8+273</f>
+        <v>279.8</v>
+      </c>
+      <c r="T6" s="2">
         <v>1.1850000000000001</v>
       </c>
-      <c r="T6" s="2">
+      <c r="U6" s="2">
         <v>1.2250000000000001</v>
       </c>
-      <c r="U6" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="V6" s="2" t="s">
-        <v>43</v>
+      <c r="V6" s="2">
+        <v>0.75</v>
       </c>
       <c r="W6" s="2">
-        <v>0.75</v>
+        <v>0.6</v>
       </c>
       <c r="X6" s="2">
-        <v>0.6</v>
+        <v>0.18</v>
       </c>
       <c r="Y6" s="2">
-        <v>0.18</v>
+        <v>0.5</v>
       </c>
       <c r="Z6" s="2">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="2">
-        <v>0</v>
+        <v>9.81</v>
       </c>
       <c r="AB6" s="2">
-        <v>9.81</v>
+        <v>3</v>
       </c>
       <c r="AC6" s="2">
-        <v>3</v>
+        <v>0.12</v>
       </c>
       <c r="AD6" s="2">
-        <v>0.12</v>
+        <v>3.3</v>
       </c>
       <c r="AE6" s="2">
-        <v>3.3</v>
+        <v>1</v>
       </c>
       <c r="AF6" s="2">
-        <v>1</v>
+        <v>1E-4</v>
       </c>
       <c r="AG6" s="2">
-        <v>1E-4</v>
-      </c>
-      <c r="AH6" s="2" t="s">
-        <v>43</v>
+        <v>0.4</v>
+      </c>
+      <c r="AH6" s="2">
+        <v>0.42</v>
       </c>
       <c r="AI6" s="2">
         <v>0.4</v>
@@ -1356,7 +1380,7 @@
         <v>2.5499999999999998</v>
       </c>
       <c r="AM6" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="AN6" s="2">
         <v>0.97</v>
@@ -1370,73 +1394,79 @@
       <c r="AQ6" s="2">
         <v>20000</v>
       </c>
+      <c r="AR6" s="2">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AD7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AL7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN7" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP7" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="AQ7" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="P7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AE7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="AL7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AP7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AQ7" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update & new code for b5
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\Mô hình hoá\Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\binh1\OneDrive\Desktop\Binh\HK3\MHH\BTL\team\Mathematical_Modelling_Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2664BB11-E437-40CA-9460-C1268796BDC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="6228"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
     <t>capCO2Top</t>
   </si>
@@ -202,12 +201,15 @@
   </si>
   <si>
     <t>nRoof_Thr</t>
+  </si>
+  <si>
+    <t>LAI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -535,52 +537,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AR7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AJ6" sqref="AI2:AJ6"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" style="2" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="2" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="6.88671875" style="2" customWidth="1"/>
     <col min="11" max="11" width="9" style="2" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" style="2" customWidth="1"/>
-    <col min="13" max="14" width="7.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" style="2" customWidth="1"/>
+    <col min="13" max="14" width="7.6640625" style="2" customWidth="1"/>
     <col min="15" max="15" width="8" style="2" customWidth="1"/>
-    <col min="16" max="16" width="18.28515625" style="2" customWidth="1"/>
-    <col min="17" max="18" width="7.140625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" style="2" customWidth="1"/>
+    <col min="17" max="18" width="7.109375" style="2" customWidth="1"/>
     <col min="19" max="19" width="7" style="2" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="2" customWidth="1"/>
-    <col min="21" max="21" width="6.5703125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="6.44140625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="6.5546875" style="2" customWidth="1"/>
     <col min="22" max="22" width="6" style="2" customWidth="1"/>
-    <col min="23" max="23" width="7.42578125" style="2" customWidth="1"/>
-    <col min="24" max="24" width="7.140625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="7.85546875" style="2" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" style="2"/>
-    <col min="27" max="27" width="6.5703125" style="2" customWidth="1"/>
-    <col min="28" max="28" width="12.28515625" style="2" customWidth="1"/>
-    <col min="29" max="29" width="7.42578125" style="2" customWidth="1"/>
-    <col min="30" max="33" width="9.140625" style="2"/>
-    <col min="34" max="36" width="10.140625" style="2" customWidth="1"/>
-    <col min="37" max="37" width="13.5703125" style="2" customWidth="1"/>
-    <col min="38" max="38" width="14.140625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="7.44140625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="7.109375" style="2" customWidth="1"/>
+    <col min="25" max="25" width="7.88671875" style="2" customWidth="1"/>
+    <col min="26" max="26" width="9.109375" style="2"/>
+    <col min="27" max="27" width="6.5546875" style="2" customWidth="1"/>
+    <col min="28" max="28" width="12.33203125" style="2" customWidth="1"/>
+    <col min="29" max="29" width="7.44140625" style="2" customWidth="1"/>
+    <col min="30" max="33" width="9.109375" style="2"/>
+    <col min="34" max="36" width="10.109375" style="2" customWidth="1"/>
+    <col min="37" max="37" width="13.5546875" style="2" customWidth="1"/>
+    <col min="38" max="38" width="14.109375" style="2" customWidth="1"/>
     <col min="39" max="39" width="10" style="2" customWidth="1"/>
-    <col min="40" max="42" width="9.140625" style="2"/>
+    <col min="40" max="42" width="9.109375" style="2"/>
     <col min="43" max="43" width="10" style="2" customWidth="1"/>
-    <col min="44" max="16384" width="9.140625" style="2"/>
+    <col min="44" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>34</v>
       </c>
@@ -710,8 +712,11 @@
       <c r="AQ1" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="AR1" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -844,8 +849,11 @@
       <c r="AQ2" s="2">
         <v>20000</v>
       </c>
+      <c r="AR2" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>35</v>
       </c>
@@ -977,8 +985,11 @@
       <c r="AQ3" s="2">
         <v>20000</v>
       </c>
+      <c r="AR3" s="2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>36</v>
       </c>
@@ -1032,8 +1043,7 @@
         <v>279</v>
       </c>
       <c r="R4" s="2">
-        <f>15.7+273</f>
-        <v>288.7</v>
+        <v>278.39999999999998</v>
       </c>
       <c r="S4" s="2">
         <f xml:space="preserve"> 6+273</f>
@@ -1111,8 +1121,11 @@
       <c r="AQ4" s="2">
         <v>20000</v>
       </c>
+      <c r="AR4" s="2">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>36</v>
       </c>
@@ -1166,8 +1179,7 @@
         <v>279.8</v>
       </c>
       <c r="R5" s="2">
-        <f>15.7+273</f>
-        <v>288.7</v>
+        <v>296.89999999999998</v>
       </c>
       <c r="S5" s="2">
         <f>6.8+273</f>
@@ -1245,8 +1257,11 @@
       <c r="AQ5" s="2">
         <v>20000</v>
       </c>
+      <c r="AR5" s="2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
@@ -1379,8 +1394,11 @@
       <c r="AQ6" s="2">
         <v>20000</v>
       </c>
+      <c r="AR6" s="2">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
         <v>54</v>
       </c>

</xml_diff>